<commit_message>
feat(feature/createDatabase): schema.sql and data.sql prototypes are added
</commit_message>
<xml_diff>
--- a/src/main/resources/static/hodgepodge_cards.xlsx
+++ b/src/main/resources/static/hodgepodge_cards.xlsx
@@ -12,9 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="7290" windowHeight="3495"/>
   </bookViews>
   <sheets>
-    <sheet name="MerchantCards" sheetId="1" r:id="rId1"/>
-    <sheet name="MixtureCards" sheetId="2" r:id="rId2"/>
-    <sheet name="KitchenCards" sheetId="3" r:id="rId3"/>
+    <sheet name="Merchant" sheetId="1" r:id="rId1"/>
+    <sheet name="Mixture" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
   <si>
     <t>Card type</t>
   </si>
@@ -76,15 +75,6 @@
     <t>Ingredients</t>
   </si>
   <si>
-    <t>KitchenCardNumber</t>
-  </si>
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>Limit</t>
-  </si>
-  <si>
     <t>R&lt;M&lt;F&lt;C</t>
   </si>
   <si>
@@ -286,16 +276,10 @@
     <t>RMFCCC</t>
   </si>
   <si>
-    <t>Starter</t>
-  </si>
-  <si>
-    <t>RRRM</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>R="root" M="mushroom" F="feather" C="chickenLeg"</t>
+  </si>
+  <si>
+    <t>list&lt;Mechant&gt; inHand</t>
   </si>
 </sst>
 </file>
@@ -703,7 +687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +698,7 @@
     <col min="4" max="4" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
@@ -740,13 +724,13 @@
         <v>9</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -767,8 +751,8 @@
       <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>88</v>
+      <c r="G2" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -789,8 +773,8 @@
       <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>88</v>
+      <c r="G3" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -801,7 +785,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5">
         <f>-3+4</f>
@@ -820,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -843,7 +827,7 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -862,7 +846,7 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
@@ -916,10 +900,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5">
         <f>-6+6+2</f>
@@ -938,10 +922,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5">
         <f>-6+4+2+2</f>
@@ -960,10 +944,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5">
         <f>-4+3+3</f>
@@ -982,10 +966,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5">
         <f>-4+3+3</f>
@@ -1004,10 +988,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5">
         <f>-6+6+2</f>
@@ -1026,10 +1010,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5">
         <f>-4+4+2</f>
@@ -1051,7 +1035,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="5">
         <f>-4+6</f>
@@ -1071,7 +1055,7 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4">
         <v>4</v>
@@ -1109,7 +1093,7 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4">
         <v>4</v>
@@ -1128,7 +1112,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4">
         <v>4</v>
@@ -1147,7 +1131,7 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
@@ -1168,7 +1152,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D22" s="5">
         <f>-2+3</f>
@@ -1187,10 +1171,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D23" s="5">
         <f>-2-1+4</f>
@@ -1209,10 +1193,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D24" s="5">
         <f>-3+4</f>
@@ -1231,10 +1215,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" s="5">
         <f>-4+4+2</f>
@@ -1256,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="5">
         <f>-3+2+3</f>
@@ -1275,10 +1259,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D27" s="5">
         <f>-6+4+4</f>
@@ -1297,10 +1281,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5">
         <f>-6+4+3+1</f>
@@ -1319,10 +1303,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D29" s="5">
         <f>-4+2+2+2</f>
@@ -1341,10 +1325,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D30" s="5">
         <f>-6+8</f>
@@ -1363,10 +1347,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D31" s="5">
         <f>-4+3+2+1</f>
@@ -1385,10 +1369,10 @@
         <v>13</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5">
         <f>-3+4+1</f>
@@ -1407,10 +1391,10 @@
         <v>13</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D33" s="5">
         <f>-3+2+4</f>
@@ -1432,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D34" s="5">
         <f>-5+8</f>
@@ -1454,7 +1438,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D35" s="5">
         <f>-4+3+4</f>
@@ -1473,10 +1457,10 @@
         <v>13</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D36" s="5">
         <f>-4-4+3+3+6</f>
@@ -1495,10 +1479,10 @@
         <v>13</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D37" s="5">
         <f>-8+9+2+1</f>
@@ -1520,7 +1504,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D38" s="5">
         <f>-5+9</f>
@@ -1539,10 +1523,10 @@
         <v>13</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D39" s="5">
         <f>-3-2+4+4</f>
@@ -1561,10 +1545,10 @@
         <v>13</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D40" s="5">
         <f>-9+4+4+4</f>
@@ -1583,10 +1567,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D41" s="5">
         <f>-6+9</f>
@@ -1608,7 +1592,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D42" s="5">
         <f>-3+6</f>
@@ -1630,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D43" s="5">
         <f>-2+4</f>
@@ -1649,10 +1633,10 @@
         <v>13</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D44" s="5">
         <f>-6+8</f>
@@ -1671,10 +1655,10 @@
         <v>13</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D45" s="5">
         <f>-4+6</f>
@@ -1693,10 +1677,10 @@
         <v>13</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D46" s="5">
         <f>-4+6</f>
@@ -1726,7 +1710,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -1751,18 +1735,18 @@
         <v>14</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4">
         <v>6</v>
@@ -1776,7 +1760,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" s="4">
         <v>7</v>
@@ -1790,7 +1774,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
@@ -1804,7 +1788,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
@@ -1817,7 +1801,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
@@ -1831,7 +1815,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" s="4">
         <v>9</v>
@@ -1845,7 +1829,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8" s="4">
         <v>10</v>
@@ -1859,7 +1843,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="4">
         <v>10</v>
@@ -1872,7 +1856,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="4">
         <v>10</v>
@@ -1886,7 +1870,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4">
         <v>11</v>
@@ -1900,7 +1884,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
@@ -1914,7 +1898,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
@@ -1927,7 +1911,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B14" s="4">
         <v>12</v>
@@ -1941,7 +1925,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" s="4">
         <v>12</v>
@@ -1955,7 +1939,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B16" s="4">
         <v>13</v>
@@ -1969,7 +1953,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4">
         <v>14</v>
@@ -1983,7 +1967,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" s="4">
         <v>14</v>
@@ -1997,7 +1981,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="4">
         <v>14</v>
@@ -2011,7 +1995,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4">
         <v>15</v>
@@ -2025,7 +2009,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4">
         <v>16</v>
@@ -2039,7 +2023,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="4">
         <v>16</v>
@@ -2053,7 +2037,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="4">
         <v>17</v>
@@ -2067,7 +2051,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="4">
         <v>18</v>
@@ -2081,7 +2065,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B25" s="4">
         <v>20</v>
@@ -2095,7 +2079,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" s="5">
         <v>9</v>
@@ -2109,7 +2093,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B27" s="5">
         <v>12</v>
@@ -2123,7 +2107,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B28" s="5">
         <v>12</v>
@@ -2137,7 +2121,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B29" s="5">
         <v>13</v>
@@ -2151,7 +2135,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B30" s="5">
         <v>15</v>
@@ -2165,7 +2149,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B31" s="5">
         <v>17</v>
@@ -2179,7 +2163,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B32" s="5">
         <v>19</v>
@@ -2193,7 +2177,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="6">
         <v>12</v>
@@ -2207,7 +2191,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B34" s="6">
         <v>14</v>
@@ -2221,7 +2205,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B35" s="6">
         <v>16</v>
@@ -2235,7 +2219,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B36" s="6">
         <v>18</v>
@@ -2249,7 +2233,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B37" s="6">
         <v>20</v>
@@ -2268,110 +2252,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>